<commit_message>
Add habitats for P01_2
</commit_message>
<xml_diff>
--- a/analysis/metadata/P01_2/P01_2_minimal_metadata.xlsx
+++ b/analysis/metadata/P01_2/P01_2_minimal_metadata.xlsx
@@ -461,6 +461,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>91D0</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>ilsø</t>
@@ -494,6 +499,21 @@
       <c r="M2" t="inlineStr">
         <is>
           <t>2018-07-11</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Bog woodland</t>
         </is>
       </c>
     </row>
@@ -519,6 +539,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>91E0</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>havkær skov</t>
@@ -552,6 +577,21 @@
       <c r="M3" t="inlineStr">
         <is>
           <t>2018-08-01</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Alluvial woodland</t>
         </is>
       </c>
     </row>
@@ -577,6 +617,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>91E0</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>karls mølle bæk</t>
@@ -610,6 +655,21 @@
       <c r="M4" t="inlineStr">
         <is>
           <t>2018-08-15</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Alluvial woodland</t>
         </is>
       </c>
     </row>
@@ -635,6 +695,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>9990</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>senderkær bæk</t>
@@ -668,6 +733,21 @@
       <c r="M5" t="inlineStr">
         <is>
           <t>2018-07-18</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Forest (non-habitattype)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Deciduous trees (løvtræer)</t>
         </is>
       </c>
     </row>
@@ -693,6 +773,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>oerum</t>
@@ -726,6 +811,21 @@
       <c r="M6" t="inlineStr">
         <is>
           <t>2018-08-07</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Forest (non-habitattype)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Willow</t>
         </is>
       </c>
     </row>
@@ -751,6 +851,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>91D0</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>skærbækvej</t>
@@ -784,6 +889,21 @@
       <c r="M7" t="inlineStr">
         <is>
           <t>2018-07-10</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Bog woodland</t>
         </is>
       </c>
     </row>
@@ -809,6 +929,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>kongensbro</t>
@@ -842,6 +967,21 @@
       <c r="M8" t="inlineStr">
         <is>
           <t>2018-08-06</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Forest (non-habitattype)</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Willow</t>
         </is>
       </c>
     </row>
@@ -867,6 +1007,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>tistedvej</t>
@@ -900,6 +1045,21 @@
       <c r="M9" t="inlineStr">
         <is>
           <t>2018-08-01</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Forest (non-habitattype)</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Willow</t>
         </is>
       </c>
     </row>
@@ -925,6 +1085,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>kielstrup sø</t>
@@ -958,6 +1123,21 @@
       <c r="M10" t="inlineStr">
         <is>
           <t>2018-07-18</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -983,6 +1163,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>østerkær</t>
@@ -1016,6 +1201,21 @@
       <c r="M11" t="inlineStr">
         <is>
           <t>2018-07-12</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -1041,6 +1241,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>havndalsvej</t>
@@ -1074,6 +1279,21 @@
       <c r="M12" t="inlineStr">
         <is>
           <t>2018-07-12</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1099,6 +1319,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>fosevej</t>
@@ -1132,6 +1357,21 @@
       <c r="M13" t="inlineStr">
         <is>
           <t>2018-07-12</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -1157,6 +1397,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>sem</t>
@@ -1190,6 +1435,21 @@
       <c r="M14" t="inlineStr">
         <is>
           <t>2018-07-18</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1215,6 +1475,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
           <t>kærby</t>
@@ -1248,6 +1513,21 @@
       <c r="M15" t="inlineStr">
         <is>
           <t>2018-07-19</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -1273,6 +1553,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>oeslanggaard</t>
@@ -1306,6 +1591,21 @@
       <c r="M16" t="inlineStr">
         <is>
           <t>2018-07-19</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1331,6 +1631,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>rejstrup</t>
@@ -1364,6 +1669,21 @@
       <c r="M17" t="inlineStr">
         <is>
           <t>2018-07-16</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1389,6 +1709,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>91D0</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>vinborgvej</t>
@@ -1422,6 +1747,21 @@
       <c r="M18" t="inlineStr">
         <is>
           <t>2018-08-08</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Bog woodland</t>
         </is>
       </c>
     </row>
@@ -1447,6 +1787,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
           <t>noerreaastien</t>
@@ -1480,6 +1825,21 @@
       <c r="M19" t="inlineStr">
         <is>
           <t>2018-08-15</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1505,6 +1865,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>7007</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>løvskal landevej</t>
@@ -1538,6 +1903,21 @@
       <c r="M20" t="inlineStr">
         <is>
           <t>2018-07-20</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Fen wetland (non-habitat type)</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Wet fens</t>
         </is>
       </c>
     </row>
@@ -1563,6 +1943,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>7007</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr">
         <is>
           <t>vinkelvej</t>
@@ -1596,6 +1981,21 @@
       <c r="M21" t="inlineStr">
         <is>
           <t>2018-07-10</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Fen wetland (non-habitat type)</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Wet fens</t>
         </is>
       </c>
     </row>
@@ -1621,6 +2021,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr">
         <is>
           <t>gudenå engene</t>
@@ -1654,6 +2059,21 @@
       <c r="M22" t="inlineStr">
         <is>
           <t>2018-07-09</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -1679,6 +2099,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr">
         <is>
           <t>lykkedalsvej</t>
@@ -1712,6 +2137,21 @@
       <c r="M23" t="inlineStr">
         <is>
           <t>2018-07-19</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -1737,6 +2177,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
         <is>
           <t>iverskilde</t>
@@ -1770,6 +2215,21 @@
       <c r="M24" t="inlineStr">
         <is>
           <t>2018-07-09</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -1795,6 +2255,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
           <t>allingaa</t>
@@ -1828,6 +2293,21 @@
       <c r="M25" t="inlineStr">
         <is>
           <t>2018-07-18</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -1853,6 +2333,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
           <t>truesoe</t>
@@ -1886,6 +2371,21 @@
       <c r="M26" t="inlineStr">
         <is>
           <t>2018-08-06</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -1911,6 +2411,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>7230</t>
+        </is>
+      </c>
       <c r="G27" t="inlineStr">
         <is>
           <t>barsbel</t>
@@ -1944,6 +2449,21 @@
       <c r="M27" t="inlineStr">
         <is>
           <t>2018-07-20</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Calcareous fens</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Alkaline fens</t>
         </is>
       </c>
     </row>
@@ -1969,6 +2489,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>91D0</t>
+        </is>
+      </c>
       <c r="G28" t="inlineStr">
         <is>
           <t>rindsholm</t>
@@ -2002,6 +2527,21 @@
       <c r="M28" t="inlineStr">
         <is>
           <t>2018-07-16</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>Bog woodland</t>
         </is>
       </c>
     </row>
@@ -2027,6 +2567,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G29" t="inlineStr">
         <is>
           <t>narren</t>
@@ -2060,6 +2605,21 @@
       <c r="M29" t="inlineStr">
         <is>
           <t>2018-07-13</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -2085,6 +2645,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G30" t="inlineStr">
         <is>
           <t>vasevej</t>
@@ -2118,6 +2683,21 @@
       <c r="M30" t="inlineStr">
         <is>
           <t>2018-07-13</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -2143,6 +2723,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>91D0</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr">
         <is>
           <t>nedenskov</t>
@@ -2176,6 +2761,21 @@
       <c r="M31" t="inlineStr">
         <is>
           <t>2018-07-17</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Temperate forests</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>Bog woodland</t>
         </is>
       </c>
     </row>
@@ -2201,6 +2801,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G32" t="inlineStr">
         <is>
           <t>stokbjergvej</t>
@@ -2234,6 +2839,21 @@
       <c r="M32" t="inlineStr">
         <is>
           <t>2018-07-11</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -2259,6 +2879,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>ajstrup</t>
@@ -2292,6 +2917,21 @@
       <c r="M33" t="inlineStr">
         <is>
           <t>2018-08-03</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -2317,6 +2957,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>7140</t>
+        </is>
+      </c>
       <c r="G34" t="inlineStr">
         <is>
           <t>fasterholt</t>
@@ -2350,6 +2995,21 @@
       <c r="M34" t="inlineStr">
         <is>
           <t>2018-08-03</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Sphagnum acid bogs</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>Quaking bogs</t>
         </is>
       </c>
     </row>
@@ -2375,6 +3035,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>9920</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
           <t>hygildvej</t>
@@ -2408,6 +3073,21 @@
       <c r="M35" t="inlineStr">
         <is>
           <t>2018-07-31</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Forests</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>Forest (non-habitattype)</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Willow</t>
         </is>
       </c>
     </row>
@@ -2433,6 +3113,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>6410</t>
+        </is>
+      </c>
       <c r="G36" t="inlineStr">
         <is>
           <t>kølvrå mose</t>
@@ -2466,6 +3151,21 @@
       <c r="M36" t="inlineStr">
         <is>
           <t>2018-08-02</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Molinia meadows</t>
         </is>
       </c>
     </row>
@@ -2491,6 +3191,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
         <is>
           <t>nederstorp</t>
@@ -2524,6 +3229,21 @@
       <c r="M37" t="inlineStr">
         <is>
           <t>2018-08-07</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -2549,6 +3269,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>7900</t>
+        </is>
+      </c>
       <c r="G38" t="inlineStr">
         <is>
           <t>toksvigvej</t>
@@ -2582,6 +3307,21 @@
       <c r="M38" t="inlineStr">
         <is>
           <t>2018-08-09</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>§3 mire</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>§3 mire</t>
         </is>
       </c>
     </row>
@@ -2607,6 +3347,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>7900</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr">
         <is>
           <t>hegildgårdvej</t>
@@ -2640,6 +3385,21 @@
       <c r="M39" t="inlineStr">
         <is>
           <t>2018-08-09</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Bogs, mires and fens</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>§3 mire</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>§3 mire</t>
         </is>
       </c>
     </row>
@@ -2665,6 +3425,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G40" t="inlineStr">
         <is>
           <t>kilderis</t>
@@ -2698,6 +3463,21 @@
       <c r="M40" t="inlineStr">
         <is>
           <t>2018-08-09</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -2723,6 +3503,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G41" t="inlineStr">
         <is>
           <t>herningmotervejen</t>
@@ -2756,6 +3541,21 @@
       <c r="M41" t="inlineStr">
         <is>
           <t>2018-07-31</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -2781,6 +3581,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G42" t="inlineStr">
         <is>
           <t>åhusevej</t>
@@ -2814,6 +3619,21 @@
       <c r="M42" t="inlineStr">
         <is>
           <t>2018-08-02</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -2839,6 +3659,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>6403</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
         <is>
           <t>torpvej</t>
@@ -2872,6 +3697,21 @@
       <c r="M43" t="inlineStr">
         <is>
           <t>2018-08-02</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Agricultural meadow (6430 subtype)</t>
         </is>
       </c>
     </row>
@@ -2897,6 +3737,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G44" t="inlineStr">
         <is>
           <t>karupvej</t>
@@ -2930,6 +3775,21 @@
       <c r="M44" t="inlineStr">
         <is>
           <t>2018-08-08</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>
@@ -2955,6 +3815,11 @@
           <t>natural_soil</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>6402</t>
+        </is>
+      </c>
       <c r="G45" t="inlineStr">
         <is>
           <t>østergaard</t>
@@ -2988,6 +3853,21 @@
       <c r="M45" t="inlineStr">
         <is>
           <t>2018-08-01</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Grassland formations</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Semi-natural tall-herb humid meadows</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Natural meadow (6410 subtype)</t>
         </is>
       </c>
     </row>

</xml_diff>